<commit_message>
fixed the scale for hair
</commit_message>
<xml_diff>
--- a/results/reports/Annotations.xlsx
+++ b/results/reports/Annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/markk_itu_dk/Documents/DS Project/PreliminaryProjectInDataScience2026/results/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="11_F25DC773A252ABDACC10489E011E5EF45ADE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB2D404B-5710-499E-AC8D-4E8C0CBCA0CF}"/>
+  <xr:revisionPtr revIDLastSave="342" documentId="11_F25DC773A252ABDACC10489E011E5EF45ADE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC09B8C5-8CA0-4927-A485-AE3A052C0245}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5430" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -951,7 +951,7 @@
         <v>20</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -993,7 +993,7 @@
         <v>23</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         <v>28</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1133,7 +1133,7 @@
         <v>33</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1161,7 +1161,7 @@
         <v>35</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1175,7 +1175,7 @@
         <v>36</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1259,7 +1259,7 @@
         <v>42</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1301,7 +1301,7 @@
         <v>45</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1371,7 +1371,7 @@
         <v>50</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>55</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>57</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>58</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>61</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         <v>63</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -1833,7 +1833,7 @@
         <v>83</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -1847,7 +1847,7 @@
         <v>84</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2029,7 +2029,7 @@
         <v>97</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -2057,7 +2057,7 @@
         <v>99</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -2085,7 +2085,7 @@
         <v>101</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2099,7 +2099,7 @@
         <v>102</v>
       </c>
       <c r="C95">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2113,7 +2113,7 @@
         <v>103</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2169,7 +2169,7 @@
         <v>107</v>
       </c>
       <c r="C100">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -2183,7 +2183,7 @@
         <v>108</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -2351,7 +2351,7 @@
         <v>120</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -2379,7 +2379,7 @@
         <v>122</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -2407,7 +2407,7 @@
         <v>124</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D117">
         <v>0</v>

</xml_diff>